<commit_message>
Updated Failed test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkUploadAdhocTnx_GBAccount.xlsx
+++ b/src/main/resources/BulkUploadAdhocTnx_GBAccount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24430" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24436" uniqueCount="682">
   <si>
     <t>transactionName</t>
   </si>
@@ -2049,6 +2049,18 @@
   <si>
     <t>7.26 AM</t>
   </si>
+  <si>
+    <t>tran8962415074</t>
+  </si>
+  <si>
+    <t>transaction18962415074</t>
+  </si>
+  <si>
+    <t>3628797091</t>
+  </si>
+  <si>
+    <t>12.37 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2721,10 +2733,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>99</v>
@@ -2784,7 +2796,7 @@
         <v>106</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>108</v>
@@ -2982,10 +2994,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>99</v>
@@ -3009,7 +3021,7 @@
         <v>106</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>108</v>

</xml_diff>